<commit_message>
icons und neues spiel - kleine änderungen
</commit_message>
<xml_diff>
--- a/Documents/Project_Management/expenditure_of_time.xlsx
+++ b/Documents/Project_Management/expenditure_of_time.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="22">
   <si>
     <t>date</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>technology decision, phonegap prototype development, server core functionality development</t>
+  </si>
+  <si>
+    <t>GUI development</t>
   </si>
 </sst>
 </file>
@@ -432,11 +435,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,6 +630,29 @@
       </c>
       <c r="H7" s="3" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>41689</v>
+      </c>
+      <c r="B9" s="2">
+        <v>4</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
expenditure of time - 14.3.14 Treffen
</commit_message>
<xml_diff>
--- a/Documents/Project_Management/expenditure_of_time.xlsx
+++ b/Documents/Project_Management/expenditure_of_time.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="29">
   <si>
     <t>date</t>
   </si>
@@ -119,6 +119,13 @@
 - Login Appfunktionalität (Screen &amp; Serveranbindung)
 csv import Pengu (Server)
 </t>
+  </si>
+  <si>
+    <t>login
+ addfriend
+ game-logic (answer questions from gameOverview, send roundResult)
+gameOverview encolourAllQuestions
+disable "Spielen"-button if not WaitingFor!</t>
   </si>
 </sst>
 </file>
@@ -478,11 +485,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,6 +778,29 @@
       </c>
       <c r="I12" s="5" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>41711</v>
+      </c>
+      <c r="B13" s="2">
+        <v>6</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added TODOS to expenditure of time
</commit_message>
<xml_diff>
--- a/Documents/Project_Management/expenditure_of_time.xlsx
+++ b/Documents/Project_Management/expenditure_of_time.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="75" windowWidth="22995" windowHeight="9750"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="22995" windowHeight="9690"/>
   </bookViews>
   <sheets>
     <sheet name="time costs" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="31">
   <si>
     <t>date</t>
   </si>
@@ -126,6 +126,23 @@
  game-logic (answer questions from gameOverview, send roundResult)
 gameOverview encolourAllQuestions
 disable "Spielen"-button if not WaitingFor!</t>
+  </si>
+  <si>
+    <t>Graue Vierecke anstatt "Verdeckt"
+Spielaufgabe disabled Spielen button bei gegner</t>
+  </si>
+  <si>
+    <t>Buttons nur auslösen, wenn Anfang &amp; ende des toches drauf sind!
+RandomEnemy (serverseitig!)
+Bei SpielEnde Benachrichtigung &amp; Ändern des SpielenButtons
+Logo anzeigen (inapp &amp; icon!)
+Frage Buttons schrift zu klein nach Auswertung!
+Beendete Spiele (letzte 5) in Sync mit liefern &amp; in Hauptmenü anzeigen.
+Duellanfragen werden u.U mehrmals im Hauptmenü angezeigt! (popUp)
+tastaturinput-enter --&gt; Aktion auf screen! (login/suchen..)
+weiterbutton durch swipe ersetzen
+login führt manchmal nicht zum home screen
+aktualisieren buttons in RÜ &amp; home in navigationbar</t>
   </si>
 </sst>
 </file>
@@ -485,11 +502,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,7 +517,7 @@
     <col min="4" max="4" width="6" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="50.140625" style="4" customWidth="1"/>
     <col min="8" max="8" width="50.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="67.42578125" style="4" customWidth="1"/>
     <col min="10" max="10" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
@@ -801,6 +818,29 @@
       </c>
       <c r="H13" s="6" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="255" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>41716</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Done for today.
</commit_message>
<xml_diff>
--- a/Documents/Project_Management/expenditure_of_time.xlsx
+++ b/Documents/Project_Management/expenditure_of_time.xlsx
@@ -128,10 +128,6 @@
 disable "Spielen"-button if not WaitingFor!</t>
   </si>
   <si>
-    <t>Graue Vierecke anstatt "Verdeckt"
-Spielaufgabe disabled Spielen button bei gegner</t>
-  </si>
-  <si>
     <t>Buttons nur auslösen, wenn Anfang &amp; ende des toches drauf sind!
 RandomEnemy (serverseitig!)
 Bei SpielEnde Benachrichtigung &amp; Ändern des SpielenButtons
@@ -143,6 +139,11 @@
 weiterbutton durch swipe ersetzen
 login führt manchmal nicht zum home screen
 aktualisieren buttons in RÜ &amp; home in navigationbar</t>
+  </si>
+  <si>
+    <t>Graue Vierecke anstatt "Verdeckt"
+Spielaufgabe disabled Spielen button bei gegner
+Server liefert 5 letzte Spiele (beendet und aufgegeben)</t>
   </si>
 </sst>
 </file>
@@ -506,7 +507,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -837,10 +838,10 @@
         <v>6</v>
       </c>
       <c r="G14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Done akutaliesiert + offene Punkte ergänzt
</commit_message>
<xml_diff>
--- a/Documents/Project_Management/expenditure_of_time.xlsx
+++ b/Documents/Project_Management/expenditure_of_time.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="32">
   <si>
     <t>date</t>
   </si>
@@ -128,6 +128,22 @@
 disable "Spielen"-button if not WaitingFor!</t>
   </si>
   <si>
+    <t>Graue Vierecke anstatt "Verdeckt"
+Spielaufgabe disabled Spielen button bei gegner
+App speichert random categories pro Runde für sich, um nicht mit Zurück-Vor-Navigation wieder neue Kategorien zu bekommen.
+Server liefert 5 letzte Spiele (beendet und aufgegeben)
+Login functioniert nun (führte manchmal nicht zum home screen)
+Workaround für Duellanfragen werden u.U mehrmals im Hauptmenü angezeigt! (popUp) wurde implementiert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zu Beachten: 
+1. Anzahl der Serveraufrufe beschränken, wichtig für späteren verlauf
+(Mögliche Überlastung des Servers)
+2. Einseitig Funktion von Steroids vermeiden (Bild in Titelzeile ist nicht für Android verfügbar) 
+Zu Besprechen: weitere Aufgabenverteilung, was wollen wir noch implementieren/was brauchen wir noch für den Prototyp
+</t>
+  </si>
+  <si>
     <t>Buttons nur auslösen, wenn Anfang &amp; ende des toches drauf sind!
 RandomEnemy (serverseitig!)
 Bei SpielEnde Benachrichtigung &amp; Ändern des SpielenButtons
@@ -137,14 +153,8 @@
 Duellanfragen werden u.U mehrmals im Hauptmenü angezeigt! (popUp)
 tastaturinput-enter --&gt; Aktion auf screen! (login/suchen..)
 weiterbutton durch swipe ersetzen
-login führt manchmal nicht zum home screen
-aktualisieren buttons in RÜ &amp; home in navigationbar</t>
-  </si>
-  <si>
-    <t>Graue Vierecke anstatt "Verdeckt"
-Spielaufgabe disabled Spielen button bei gegner
-App speichert random categories pro Runde für sich, um nicht mit Zurück-Vor-Navigation wieder neue Kategorien zu bekommen.
-Server liefert 5 letzte Spiele (beendet und aufgegeben)</t>
+aktualisieren buttons in RÜ &amp; home in navigationbar
+Präsentation</t>
   </si>
 </sst>
 </file>
@@ -508,7 +518,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
+      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,7 +832,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="255" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="285" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>41716</v>
       </c>
@@ -839,10 +849,13 @@
         <v>6</v>
       </c>
       <c r="G14" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I14" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>